<commit_message>
benchmarks coming along nicely
</commit_message>
<xml_diff>
--- a/latex/gpu_content/cascade_spmv/spmv_benchmarks.xlsx
+++ b/latex/gpu_content/cascade_spmv/spmv_benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14920" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="m2070_n17" sheetId="2" r:id="rId1"/>
@@ -766,6 +766,1759 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>GFLOP/s M2070 (n=101)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>m2070_n101!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>COO_CPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2562.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10201.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10242.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27556.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40962.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>163842.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>m2070_n101!$H$6:$H$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.253117480191725</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26861632361535</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.175208275330349</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17449272171461</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.173247249158418</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.187526871972122</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.168524449207834</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.170115317797264</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.162201703439078</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.164388061332446</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.154642095415704</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.151866122645126</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>m2070_n101!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>COO_GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2562.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10201.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10242.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27556.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40962.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>163842.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>m2070_n101!$I$6:$I$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.75789402173913</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.860143884892087</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.991237677984666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.061839103462078</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.021579050224741</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.073794097374522</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.147331224442558</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.209078385305425</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.158857729138167</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.164203629230015</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.19076106171656</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.177646352388458</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>m2070_n101!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CSR_GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2562.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10201.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10242.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27556.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40962.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>163842.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>m2070_n101!$J$6:$J$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.326304459251666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.622019211919232</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.693438211550404</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.712174491067719</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.687369708832885</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.750908898529256</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.741159248021521</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.505818850206555</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.523826766545213</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.707946969970636</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.720244036203472</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.658916842276428</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>m2070_n101!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ELL_GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2562.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10201.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10242.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27556.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40962.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>163842.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>m2070_n101!$K$6:$K$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2.644476239141543</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.09194856577646</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.462085308056873</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.093294320137695</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.03462767766066</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.647053625225949</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.85980231573002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.738799102132435</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.316189786309309</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.45840257586106</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.53433343528306</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.365312199656526</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2095685560"/>
+        <c:axId val="2095691048"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2095685560"/>
+        <c:scaling>
+          <c:logBase val="2.0"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1.5E6"/>
+          <c:min val="2000.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>N</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2095691048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2095691048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="32.0"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>GFLOP/s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2095685560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="4.0"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Speedup M2070 (n=101)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>m2070_n101!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>COO_CPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2562.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10201.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10242.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27556.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40962.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>163842.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>m2070_n101!$M$6:$M$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>m2070_n101!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>COO_GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2562.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10201.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10242.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27556.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40962.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>163842.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>m2070_n101!$N$6:$N$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>6.944972826086957</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.924910071942446</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.36497505172204</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.8161897138283</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.6687512214188</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.05865029137164</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.74195663914821</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.98576997009825</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.30971058481532</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.16521170508419</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.16665401375624</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.3392503506334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>m2070_n101!$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CSR_GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2562.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10201.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10242.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27556.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40962.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>163842.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>m2070_n101!$O$6:$O$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5.239876986160943</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.038423838463046</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.665286690126267</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.812297465724968</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.739662344017617</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.336842662152152</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.33179017172886</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.851753444102712</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.394640957747753</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.38972633491075</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.12403470464602</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.92354774970394</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>m2070_n101!$P$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ELL_GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2562.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10201.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10242.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27556.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40962.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>163842.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>m2070_n101!$P$6:$P$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10.44762391415432</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.23343224530168</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36.88230647709321</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.65094664371773</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.60455627337641</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.44587266519381</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>46.6389438011861</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45.49148896371118</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.10550525172039</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39.28754024782905</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>48.72110284738125</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41.91397059982038</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2095735624"/>
+        <c:axId val="2095741112"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2095735624"/>
+        <c:scaling>
+          <c:logBase val="2.0"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1.5E6"/>
+          <c:min val="2000.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>N</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2095741112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2095741112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="128.0"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Speedup (S</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="-25000"/>
+                  <a:t>p</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> = t</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="-25000"/>
+                  <a:t>CPU</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>/t</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="-25000"/>
+                  <a:t>GPU</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2095735624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time (ms) M2070 (n=101)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>m2070_n101!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>COO_CPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2562.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10201.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10242.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27556.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40962.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>163842.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>m2070_n101!$C$6:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2.0446</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0802</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.3386</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.8091</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.9418</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.6485</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.0297</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>48.6395</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>124.5363</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>201.329</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>653.121</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1330.1189</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>m2070_n101!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>COO_GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2562.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10201.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10242.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27556.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40962.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>163842.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>m2070_n101!$D$6:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.2944</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4448</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8217</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0234</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5959</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5922</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.7456</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.3568</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.2925</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46.1027</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>92.7607</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>m2070_n101!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CSR_GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2562.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10201.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10242.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27556.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40962.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>163842.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>m2070_n101!$E$6:$E$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.3902</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9662</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2035</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2261</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8902</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.1969</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.4949</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.2561</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.3777</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>58.7126</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>121.7662</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>m2070_n101!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ELL_GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2562.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10201.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10242.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27556.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40962.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>163842.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>m2070_n101!$F$6:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.1957</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2022</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2532</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2905</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2941</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4979</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7082</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0692</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.761</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.1245</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.4053</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>31.7345</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2117635176"/>
+        <c:axId val="2117640664"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2117635176"/>
+        <c:scaling>
+          <c:logBase val="2.0"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1.5E6"/>
+          <c:min val="2000.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>N</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2117640664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2117640664"/>
+        <c:scaling>
+          <c:logBase val="2.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2117635176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="4.0"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
@@ -1956,6 +3709,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>GFLOP/s M2070 (n=31)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -2394,53 +4166,104 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2095579720"/>
-        <c:axId val="2095582856"/>
+        <c:axId val="2120480376"/>
+        <c:axId val="2120485864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2095579720"/>
+        <c:axId val="2120480376"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
-          <c:min val="1024.0"/>
+          <c:max val="1.5E6"/>
+          <c:min val="2000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>N</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095582856"/>
+        <c:crossAx val="2120485864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2095582856"/>
+        <c:axId val="2120485864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32.0"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>GFLOP/s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095579720"/>
+        <c:crossAx val="2120480376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -2463,6 +4286,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Speedup M2070 (n=31)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -2474,7 +4316,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>m2070_n50!$H$2</c:f>
+              <c:f>m2070_n31!$M$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2485,7 +4327,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>m2070_n50!$B$6:$B$17</c:f>
+              <c:f>m2070_n31!$B$6:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2530,45 +4372,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>m2070_n50!$H$6:$H$17</c:f>
+              <c:f>m2070_n31!$M$6:$M$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.333951087307221</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.371778027409571</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.302104874446086</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.294999642095317</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.287073874673919</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.290687816746155</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.248162602930883</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.25431053930533</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.238542294021091</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.242206639149908</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.221729051928285</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.215912425065295</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2580,7 +4422,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>m2070_n50!$I$2</c:f>
+              <c:f>m2070_n31!$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2591,7 +4433,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>m2070_n50!$B$6:$B$17</c:f>
+              <c:f>m2070_n31!$B$6:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2636,45 +4478,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>m2070_n50!$I$6:$I$17</c:f>
+              <c:f>m2070_n31!$N$6:$N$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>2.927171945701357</c:v>
+                  <c:v>10.50542635658915</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.274206569054215</c:v>
+                  <c:v>10.86878838637633</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.636</c:v>
+                  <c:v>14.7566120906801</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.791356025758969</c:v>
+                  <c:v>15.30805812417437</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.664335812964931</c:v>
+                  <c:v>15.78279009126467</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.880370500644859</c:v>
+                  <c:v>15.46745356708905</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.093779510186071</c:v>
+                  <c:v>20.75429572069607</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.120063735497684</c:v>
+                  <c:v>21.24854606672789</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.990281097524841</c:v>
+                  <c:v>22.3020417742314</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.079188009958834</c:v>
+                  <c:v>21.96480702738062</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.18543551321313</c:v>
+                  <c:v>24.78128596224639</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.202379961720895</c:v>
+                  <c:v>25.65121321332897</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2686,7 +4528,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>m2070_n50!$J$2</c:f>
+              <c:f>m2070_n31!$O$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2697,7 +4539,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>m2070_n50!$B$6:$B$17</c:f>
+              <c:f>m2070_n31!$B$6:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2742,45 +4584,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>m2070_n50!$J$6:$J$17</c:f>
+              <c:f>m2070_n31!$O$6:$O$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>2.509815712900097</c:v>
+                  <c:v>9.700787401574804</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.029630172098132</c:v>
+                  <c:v>10.31584525702173</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.228492501973165</c:v>
+                  <c:v>13.82099675611914</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.325697224015494</c:v>
+                  <c:v>14.06676377761593</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.293876771214775</c:v>
+                  <c:v>14.67677012609117</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.423572980242061</c:v>
+                  <c:v>14.07042475919785</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.445779373529776</c:v>
+                  <c:v>18.11020914907841</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.931039319872476</c:v>
+                  <c:v>14.64072550880523</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.107118685781087</c:v>
+                  <c:v>18.04105460499775</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.452363636363636</c:v>
+                  <c:v>18.90739578808501</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.423276244835428</c:v>
+                  <c:v>20.92801301532415</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.389216252130844</c:v>
+                  <c:v>21.49907120242941</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2792,7 +4634,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>m2070_n50!$K$2</c:f>
+              <c:f>m2070_n31!$P$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2803,7 +4645,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>m2070_n50!$B$6:$B$17</c:f>
+              <c:f>m2070_n31!$B$6:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2848,45 +4690,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>m2070_n50!$K$6:$K$17</c:f>
+              <c:f>m2070_n31!$P$6:$P$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>4.323508771929824</c:v>
+                  <c:v>15.0913140311804</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.57704292527822</c:v>
+                  <c:v>19.33068520357498</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.08133086876155</c:v>
+                  <c:v>36.30286599535244</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.2724398249453</c:v>
+                  <c:v>40.60336370007008</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.08726688102894</c:v>
+                  <c:v>42.23796231681785</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.24555895344886</c:v>
+                  <c:v>40.39347234814143</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.64961255517411</c:v>
+                  <c:v>62.11333114968883</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.67882955860473</c:v>
+                  <c:v>65.12101313320827</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.06618481572188</c:v>
+                  <c:v>61.06771628243233</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.10625649279391</c:v>
+                  <c:v>58.65869727976042</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13.26503808773312</c:v>
+                  <c:v>76.20534928734822</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.86656984891335</c:v>
+                  <c:v>78.63819164754656</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2901,54 +4743,127 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2095630440"/>
-        <c:axId val="2095633576"/>
+        <c:axId val="2120523976"/>
+        <c:axId val="2120687560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2095630440"/>
+        <c:axId val="2120523976"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
-          <c:min val="1024.0"/>
+          <c:max val="1.5E6"/>
+          <c:min val="2000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>N</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095633576"/>
+        <c:crossAx val="2120687560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2095633576"/>
+        <c:axId val="2120687560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="32.0"/>
+          <c:max val="128.0"/>
           <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Speedup (S</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="-25000"/>
+                  <a:t>p</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> = t</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="-25000"/>
+                  <a:t>CPU</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>/t</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="-25000"/>
+                  <a:t>GPU</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095630440"/>
+        <c:crossAx val="2120523976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="4.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -2982,7 +4897,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>GFLOP/s M2070 (n=101)</a:t>
+              <a:t>Time (ms) M2070 (n=31)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3001,7 +4916,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>m2070_n101!$H$2</c:f>
+              <c:f>m2070_n31!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3012,7 +4927,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:f>m2070_n31!$B$6:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3057,45 +4972,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>m2070_n101!$H$6:$H$17</c:f>
+              <c:f>m2070_n31!$C$6:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.253117480191725</c:v>
+                  <c:v>1.3552</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.26861632361535</c:v>
+                  <c:v>1.9466</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.175208275330349</c:v>
+                  <c:v>4.6867</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17449272171461</c:v>
+                  <c:v>5.7941</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.173247249158418</c:v>
+                  <c:v>6.0527</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.187526871972122</c:v>
+                  <c:v>8.9108</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.168524449207834</c:v>
+                  <c:v>18.9632</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.170115317797264</c:v>
+                  <c:v>27.7676</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.162201703439078</c:v>
+                  <c:v>76.0232</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.164388061332446</c:v>
+                  <c:v>117.5227</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.154642095415704</c:v>
+                  <c:v>389.7675</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.151866122645126</c:v>
+                  <c:v>798.5787</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3107,7 +5022,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>m2070_n101!$I$2</c:f>
+              <c:f>m2070_n31!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3118,7 +5033,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:f>m2070_n31!$B$6:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3163,45 +5078,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>m2070_n101!$I$6:$I$17</c:f>
+              <c:f>m2070_n31!$D$6:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1.75789402173913</c:v>
+                  <c:v>0.129</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.860143884892087</c:v>
+                  <c:v>0.1791</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.991237677984666</c:v>
+                  <c:v>0.3176</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.061839103462078</c:v>
+                  <c:v>0.3785</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.021579050224741</c:v>
+                  <c:v>0.3835</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.073794097374522</c:v>
+                  <c:v>0.5761</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.147331224442558</c:v>
+                  <c:v>0.9137</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.209078385305425</c:v>
+                  <c:v>1.3068</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.158857729138167</c:v>
+                  <c:v>3.4088</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.164203629230015</c:v>
+                  <c:v>5.3505</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.19076106171656</c:v>
+                  <c:v>15.7283</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.177646352388458</c:v>
+                  <c:v>31.1322</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3213,7 +5128,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>m2070_n101!$J$2</c:f>
+              <c:f>m2070_n31!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3224,7 +5139,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:f>m2070_n31!$B$6:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3269,45 +5184,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>m2070_n101!$J$6:$J$17</c:f>
+              <c:f>m2070_n31!$E$6:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1.326304459251666</c:v>
+                  <c:v>0.1397</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.622019211919232</c:v>
+                  <c:v>0.1887</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.693438211550404</c:v>
+                  <c:v>0.3391</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.712174491067719</c:v>
+                  <c:v>0.4119</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.687369708832885</c:v>
+                  <c:v>0.4124</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.750908898529256</c:v>
+                  <c:v>0.6333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.741159248021521</c:v>
+                  <c:v>1.0471</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.505818850206555</c:v>
+                  <c:v>1.8966</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.523826766545213</c:v>
+                  <c:v>4.2139</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.707946969970636</c:v>
+                  <c:v>6.2157</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.720244036203472</c:v>
+                  <c:v>18.6242</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.658916842276428</c:v>
+                  <c:v>37.1448</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3319,7 +5234,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>m2070_n101!$K$2</c:f>
+              <c:f>m2070_n31!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3330,7 +5245,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:f>m2070_n31!$B$6:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3375,45 +5290,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>m2070_n101!$K$6:$K$17</c:f>
+              <c:f>m2070_n31!$F$6:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>2.644476239141543</c:v>
+                  <c:v>0.0898</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.09194856577646</c:v>
+                  <c:v>0.1007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.462085308056873</c:v>
+                  <c:v>0.1291</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.093294320137695</c:v>
+                  <c:v>0.1427</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.03462767766066</c:v>
+                  <c:v>0.1433</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.647053625225949</c:v>
+                  <c:v>0.2206</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.85980231573002</c:v>
+                  <c:v>0.3053</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.738799102132435</c:v>
+                  <c:v>0.4264</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.316189786309309</c:v>
+                  <c:v>1.2449</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.45840257586106</c:v>
+                  <c:v>2.0035</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.53433343528306</c:v>
+                  <c:v>5.1147</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.365312199656526</c:v>
+                  <c:v>10.1551</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3428,11 +5343,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2095685560"/>
-        <c:axId val="2095691048"/>
+        <c:axId val="2119035928"/>
+        <c:axId val="2119075944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2095685560"/>
+        <c:axId val="2119035928"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -3464,16 +5379,15 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095691048"/>
+        <c:crossAx val="2119075944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2095691048"/>
+        <c:axId val="2119075944"/>
         <c:scaling>
+          <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
-          <c:max val="32.0"/>
-          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3489,7 +5403,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>GFLOP/s</a:t>
+                  <a:t>Time (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3501,7 +5415,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095685560"/>
+        <c:crossAx val="2119035928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4.0"/>
@@ -3559,7 +5473,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Speedup M2070 (n=101)</a:t>
+              <a:t>GFLOP/s M2070 (n=50)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3578,7 +5492,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>m2070_n101!$M$2</c:f>
+              <c:f>m2070_n50!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3589,7 +5503,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:f>m2070_n50!$B$6:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3634,45 +5548,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>m2070_n101!$M$6:$M$17</c:f>
+              <c:f>m2070_n50!$H$6:$H$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>0.333951087307221</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>0.371778027409571</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>0.302104874446086</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>0.294999642095317</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>0.287073874673919</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0</c:v>
+                  <c:v>0.290687816746155</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0</c:v>
+                  <c:v>0.248162602930883</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0</c:v>
+                  <c:v>0.25431053930533</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0</c:v>
+                  <c:v>0.238542294021091</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0</c:v>
+                  <c:v>0.242206639149908</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0</c:v>
+                  <c:v>0.221729051928285</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0</c:v>
+                  <c:v>0.215912425065295</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3684,7 +5598,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>m2070_n101!$N$2</c:f>
+              <c:f>m2070_n50!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3695,7 +5609,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:f>m2070_n50!$B$6:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3740,45 +5654,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>m2070_n101!$N$6:$N$17</c:f>
+              <c:f>m2070_n50!$I$6:$I$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>6.944972826086957</c:v>
+                  <c:v>2.927171945701357</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.924910071942446</c:v>
+                  <c:v>3.274206569054215</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.36497505172204</c:v>
+                  <c:v>3.636</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.8161897138283</c:v>
+                  <c:v>3.791356025758969</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.6687512214188</c:v>
+                  <c:v>3.664335812964931</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.05865029137164</c:v>
+                  <c:v>3.880370500644859</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.74195663914821</c:v>
+                  <c:v>4.093779510186071</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.98576997009825</c:v>
+                  <c:v>4.120063735497684</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.30971058481532</c:v>
+                  <c:v>3.990281097524841</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.16521170508419</c:v>
+                  <c:v>4.079188009958834</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14.16665401375624</c:v>
+                  <c:v>4.18543551321313</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14.3392503506334</c:v>
+                  <c:v>4.202379961720895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3790,7 +5704,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>m2070_n101!$O$2</c:f>
+              <c:f>m2070_n50!$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3801,7 +5715,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:f>m2070_n50!$B$6:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3846,45 +5760,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>m2070_n101!$O$6:$O$17</c:f>
+              <c:f>m2070_n50!$J$6:$J$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>5.239876986160943</c:v>
+                  <c:v>2.509815712900097</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.038423838463046</c:v>
+                  <c:v>3.029630172098132</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.665286690126267</c:v>
+                  <c:v>3.228492501973165</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.812297465724968</c:v>
+                  <c:v>3.325697224015494</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.739662344017617</c:v>
+                  <c:v>3.293876771214775</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.336842662152152</c:v>
+                  <c:v>3.423572980242061</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.33179017172886</c:v>
+                  <c:v>3.445779373529776</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.851753444102712</c:v>
+                  <c:v>2.931039319872476</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.394640957747753</c:v>
+                  <c:v>3.107118685781087</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.38972633491075</c:v>
+                  <c:v>3.452363636363636</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.12403470464602</c:v>
+                  <c:v>3.423276244835428</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10.92354774970394</c:v>
+                  <c:v>3.389216252130844</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3896,7 +5810,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>m2070_n101!$P$2</c:f>
+              <c:f>m2070_n50!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3907,7 +5821,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:f>m2070_n50!$B$6:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3952,45 +5866,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>m2070_n101!$P$6:$P$17</c:f>
+              <c:f>m2070_n50!$K$6:$K$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>10.44762391415432</c:v>
+                  <c:v>4.323508771929824</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.23343224530168</c:v>
+                  <c:v>6.57704292527822</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.88230647709321</c:v>
+                  <c:v>10.08133086876155</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.65094664371773</c:v>
+                  <c:v>11.2724398249453</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.60455627337641</c:v>
+                  <c:v>11.08726688102894</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35.44587266519381</c:v>
+                  <c:v>11.24555895344886</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>46.6389438011861</c:v>
+                  <c:v>13.64961255517411</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45.49148896371118</c:v>
+                  <c:v>13.67882955860473</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45.10550525172039</c:v>
+                  <c:v>12.06618481572188</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>39.28754024782905</c:v>
+                  <c:v>12.10625649279391</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>48.72110284738125</c:v>
+                  <c:v>13.26503808773312</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>41.91397059982038</c:v>
+                  <c:v>12.86656984891335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4005,11 +5919,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2095735624"/>
-        <c:axId val="2095741112"/>
+        <c:axId val="2116132104"/>
+        <c:axId val="2116623672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2095735624"/>
+        <c:axId val="2116132104"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -4041,12 +5955,589 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095741112"/>
+        <c:crossAx val="2116623672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2095741112"/>
+        <c:axId val="2116623672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="32.0"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>GFLOP/s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2116132104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="4.0"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Speedup M2070 (n=50)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>m2070_n50!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>COO_CPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>m2070_n50!$B$6:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2562.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10201.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10242.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27556.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40962.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>163842.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>m2070_n50!$M$6:$M$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>m2070_n50!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>COO_GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>m2070_n50!$B$6:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2562.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10201.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10242.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27556.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40962.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>163842.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>m2070_n50!$N$6:$N$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>8.765271493212669</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.806885635140483</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.03555555555556</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.85206991720331</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.76443499822884</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.34892718958846</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.4963594910642</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.20091619777921</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.72777196136144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16.84176793945818</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18.87635146055123</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19.46335399850212</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>m2070_n50!$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CSR_GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>m2070_n50!$B$6:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2562.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10201.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10242.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27556.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40962.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>163842.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>m2070_n50!$O$6:$O$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>7.515518913676043</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.149029659465396</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.68666140489345</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.27356358941252</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.47396911319854</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.77749043136444</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.88516776030704</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.52543393552958</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.0254414569618</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.25379439837271</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.43900636864957</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.69718023919142</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>m2070_n50!$P$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ELL_GPU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>m2070_n50!$B$6:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2562.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10201.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10242.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16384.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27556.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40962.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>163842.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>m2070_n50!$P$6:$P$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>12.94653299916458</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.69077901430843</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.37030191004313</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38.21170678336981</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38.62165058949626</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38.68603465851172</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55.00269740068661</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>53.78789882625227</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50.58299982079924</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>49.98317360450655</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>59.82543997898607</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>59.59161379907768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2118813960"/>
+        <c:axId val="2118797000"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2118813960"/>
+        <c:scaling>
+          <c:logBase val="2.0"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1.5E6"/>
+          <c:min val="2000.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>N</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2118797000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2118797000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="128.0"/>
@@ -4102,7 +6593,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095735624"/>
+        <c:crossAx val="2118813960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4134,7 +6625,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4159,7 +6650,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Time (ms) M2070 (n=101)</a:t>
+              <a:t>Time (ms) M2070 (n=50)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4178,7 +6669,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>m2070_n101!$C$2</c:f>
+              <c:f>m2070_n50!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4189,7 +6680,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:f>m2070_n50!$B$6:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4234,45 +6725,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>m2070_n101!$C$6:$C$17</c:f>
+              <c:f>m2070_n50!$C$6:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>2.0446</c:v>
+                  <c:v>1.5497</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0802</c:v>
+                  <c:v>2.2255</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.3386</c:v>
+                  <c:v>5.416</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.8091</c:v>
+                  <c:v>6.9851</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.9418</c:v>
+                  <c:v>7.2068</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.6485</c:v>
+                  <c:v>11.3853</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.0297</c:v>
+                  <c:v>22.4301</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>48.6395</c:v>
+                  <c:v>32.5363</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>124.5363</c:v>
+                  <c:v>84.681</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>201.329</c:v>
+                  <c:v>136.644</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>653.121</c:v>
+                  <c:v>455.5109</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1330.1189</c:v>
+                  <c:v>935.5645</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4284,7 +6775,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>m2070_n101!$D$2</c:f>
+              <c:f>m2070_n50!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4295,7 +6786,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:f>m2070_n50!$B$6:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4340,45 +6831,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>m2070_n101!$D$6:$D$17</c:f>
+              <c:f>m2070_n50!$D$6:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.2944</c:v>
+                  <c:v>0.1768</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4448</c:v>
+                  <c:v>0.2527</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8217</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9994</c:v>
+                  <c:v>0.5435</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0234</c:v>
+                  <c:v>0.5646</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5959</c:v>
+                  <c:v>0.8529</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5922</c:v>
+                  <c:v>1.3597</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.7456</c:v>
+                  <c:v>2.0083</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.3568</c:v>
+                  <c:v>5.0623</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15.2925</c:v>
+                  <c:v>8.1134</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>46.1027</c:v>
+                  <c:v>24.1313</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>92.7607</c:v>
+                  <c:v>48.068</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4390,7 +6881,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>m2070_n101!$E$2</c:f>
+              <c:f>m2070_n50!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4401,7 +6892,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:f>m2070_n50!$B$6:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4446,45 +6937,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>m2070_n101!$E$6:$E$17</c:f>
+              <c:f>m2070_n50!$E$6:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.3902</c:v>
+                  <c:v>0.2062</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5101</c:v>
+                  <c:v>0.2731</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9662</c:v>
+                  <c:v>0.5068</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2035</c:v>
+                  <c:v>0.6196</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2261</c:v>
+                  <c:v>0.6281</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.8902</c:v>
+                  <c:v>0.9667</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.1969</c:v>
+                  <c:v>1.6154</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.4949</c:v>
+                  <c:v>2.823</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.2561</c:v>
+                  <c:v>6.5012</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19.3777</c:v>
+                  <c:v>9.5865</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>58.7126</c:v>
+                  <c:v>29.5039</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>121.7662</c:v>
+                  <c:v>59.6008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4496,7 +6987,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>m2070_n101!$F$2</c:f>
+              <c:f>m2070_n50!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4507,7 +6998,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>m2070_n101!$B$6:$B$17</c:f>
+              <c:f>m2070_n50!$B$6:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -4552,45 +7043,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>m2070_n101!$F$6:$F$17</c:f>
+              <c:f>m2070_n50!$F$6:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.1957</c:v>
+                  <c:v>0.1197</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2022</c:v>
+                  <c:v>0.1258</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.2532</c:v>
+                  <c:v>0.1623</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.2905</c:v>
+                  <c:v>0.1828</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.2941</c:v>
+                  <c:v>0.1866</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4979</c:v>
+                  <c:v>0.2943</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.7082</c:v>
+                  <c:v>0.4078</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0692</c:v>
+                  <c:v>0.6049</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.761</c:v>
+                  <c:v>1.6741</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.1245</c:v>
+                  <c:v>2.7338</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13.4053</c:v>
+                  <c:v>7.614</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>31.7345</c:v>
+                  <c:v>15.6996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4605,11 +7096,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2117635176"/>
-        <c:axId val="2117640664"/>
+        <c:axId val="2116590440"/>
+        <c:axId val="2118794664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2117635176"/>
+        <c:axId val="2116590440"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -4641,12 +7132,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117640664"/>
+        <c:crossAx val="2118794664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2117640664"/>
+        <c:axId val="2118794664"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -4677,7 +7168,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117635176"/>
+        <c:crossAx val="2116590440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4.0"/>
@@ -4816,19 +7307,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4845,6 +7336,70 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4853,19 +7408,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4877,6 +7432,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5308,8 +7927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="K51" sqref="K51"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6162,8 +8781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="K78" sqref="K78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7016,8 +9635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:P17"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7869,8 +10488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K56" sqref="K56"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>